<commit_message>
Fix Seeder, import excel
</commit_message>
<xml_diff>
--- a/database/seeders/data/dosen.xlsx
+++ b/database/seeders/data/dosen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="14960"/>
+    <workbookView windowHeight="14140"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>nidn</t>
   </si>
@@ -242,7 +242,7 @@
     <t>Morga Ohiwal</t>
   </si>
   <si>
-    <t>morgaohiwal@ummaluku.ac.id</t>
+    <t>morganohiwal@ummaluku.ac.id</t>
   </si>
   <si>
     <t>07</t>
@@ -288,6 +288,33 @@
   </si>
   <si>
     <t>dosen@ummaluku.ac.id</t>
+  </si>
+  <si>
+    <t>11111</t>
+  </si>
+  <si>
+    <t>Prof. Faris Al-Fadhat, M.A., Ph.D.</t>
+  </si>
+  <si>
+    <t>farisalfadhat@ummaluku.ac.id</t>
+  </si>
+  <si>
+    <t>22222</t>
+  </si>
+  <si>
+    <t>Dr. Andi Thamrin, SP., M.Si.</t>
+  </si>
+  <si>
+    <t>andithamrin@ummaluku.ac.id</t>
+  </si>
+  <si>
+    <t>33333</t>
+  </si>
+  <si>
+    <t>Dr. Imam Suprabowo, S.Sos.I., M.Pd.I.</t>
+  </si>
+  <si>
+    <t>imamsuprabowo@ummaluku.ac.id</t>
   </si>
 </sst>
 </file>
@@ -300,7 +327,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -312,6 +339,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <charset val="1"/>
       <scheme val="minor"/>
@@ -338,12 +373,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="12"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -986,150 +1019,150 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1189,6 +1222,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1197,15 +1233,17 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1269,12 +1307,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFF9900"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1566,21 +1601,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="18.1625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.45" customWidth="1"/>
-    <col min="3" max="3" width="25.2" customWidth="1"/>
-    <col min="4" max="4" width="16.825" customWidth="1"/>
+    <col min="1" max="1" width="18.1607142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.3214285714286" customWidth="1"/>
+    <col min="3" max="3" width="33.4821428571429" customWidth="1"/>
+    <col min="4" max="4" width="16.8214285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.15" spans="1:4">
+    <row r="1" ht="18.35" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1594,7 +1629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="17" spans="1:4">
+    <row r="2" ht="18" spans="1:4">
       <c r="A2" s="5">
         <v>1221048601</v>
       </c>
@@ -1608,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="17" spans="1:4">
+    <row r="3" ht="18" spans="1:4">
       <c r="A3" s="8">
         <v>1210038801</v>
       </c>
@@ -1622,7 +1657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="17" spans="1:4">
+    <row r="4" ht="18" spans="1:4">
       <c r="A4" s="11">
         <v>1208129501</v>
       </c>
@@ -1636,7 +1671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="17" spans="1:4">
+    <row r="5" ht="18" spans="1:4">
       <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
@@ -1650,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="17" spans="1:4">
+    <row r="6" ht="18" spans="1:4">
       <c r="A6" s="16" t="s">
         <v>13</v>
       </c>
@@ -1748,7 +1783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" ht="17" spans="1:4">
+    <row r="13" ht="18" spans="1:4">
       <c r="A13" s="18">
         <v>1228078512</v>
       </c>
@@ -1762,7 +1797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" ht="17" spans="1:4">
+    <row r="14" ht="18" spans="1:4">
       <c r="A14" s="20">
         <v>1216129001</v>
       </c>
@@ -1776,7 +1811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" ht="17" spans="1:4">
+    <row r="15" ht="18" spans="1:4">
       <c r="A15" s="18">
         <v>1221118201</v>
       </c>
@@ -1790,7 +1825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" ht="17" spans="1:4">
+    <row r="16" ht="18" spans="1:4">
       <c r="A16" s="20">
         <v>1205098702</v>
       </c>
@@ -1804,7 +1839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" ht="17" spans="1:4">
+    <row r="17" ht="18" spans="1:4">
       <c r="A17" s="18">
         <v>12280785122</v>
       </c>
@@ -1818,7 +1853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" ht="17" spans="1:4">
+    <row r="18" ht="18" spans="1:4">
       <c r="A18" s="16" t="s">
         <v>39</v>
       </c>
@@ -1832,7 +1867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" ht="17" spans="1:4">
+    <row r="19" ht="18" spans="1:4">
       <c r="A19" s="14" t="s">
         <v>42</v>
       </c>
@@ -1860,7 +1895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" ht="17" spans="1:4">
+    <row r="21" ht="18" spans="1:4">
       <c r="A21" s="14" t="s">
         <v>48</v>
       </c>
@@ -1874,7 +1909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" ht="17" spans="1:4">
+    <row r="22" ht="18" spans="1:4">
       <c r="A22" s="16" t="s">
         <v>51</v>
       </c>
@@ -1888,7 +1923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" ht="33" spans="1:4">
+    <row r="23" ht="18" spans="1:4">
       <c r="A23" s="14" t="s">
         <v>54</v>
       </c>
@@ -1902,7 +1937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" ht="17" spans="1:4">
+    <row r="24" ht="18" spans="1:4">
       <c r="A24" s="16" t="s">
         <v>57</v>
       </c>
@@ -1916,7 +1951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" ht="17" spans="1:4">
+    <row r="25" ht="18" spans="1:4">
       <c r="A25" s="14" t="s">
         <v>60</v>
       </c>
@@ -1930,7 +1965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" ht="17" spans="1:4">
+    <row r="26" ht="18" spans="1:4">
       <c r="A26" s="16" t="s">
         <v>63</v>
       </c>
@@ -1944,7 +1979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" ht="17" spans="1:4">
+    <row r="27" ht="18" spans="1:4">
       <c r="A27" s="14" t="s">
         <v>66</v>
       </c>
@@ -1958,101 +1993,143 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" ht="17" spans="1:4">
+    <row r="28" ht="18" spans="1:4">
       <c r="A28" s="16" t="s">
         <v>69</v>
       </c>
       <c r="B28" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="25" t="s">
         <v>71</v>
       </c>
       <c r="D28" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="29" ht="17" spans="1:4">
-      <c r="A29" s="25" t="s">
+    <row r="29" ht="18" spans="1:4">
+      <c r="A29" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="28">
+      <c r="D29" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="30" ht="16.8" spans="1:4">
-      <c r="A30" s="33" t="s">
+    <row r="30" spans="1:4">
+      <c r="A30" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="32" t="s">
         <v>77</v>
       </c>
       <c r="D30" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="31" ht="16.8" spans="1:4">
-      <c r="A31" s="33" t="s">
+    <row r="31" spans="1:4">
+      <c r="A31" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="28">
+      <c r="D31" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="32" ht="16.8" spans="1:4">
-      <c r="A32" s="29">
+    <row r="32" spans="1:4">
+      <c r="A32" s="30">
         <v>10</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="32" t="s">
         <v>82</v>
       </c>
       <c r="D32" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="33" ht="16.8" spans="1:4">
-      <c r="A33" s="29">
+    <row r="33" spans="1:4">
+      <c r="A33" s="30">
         <v>11</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="28">
+      <c r="D33" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="34" ht="16.8" spans="1:4">
-      <c r="A34" s="29">
+    <row r="34" spans="1:4">
+      <c r="A34" s="30">
         <v>12</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="31" t="s">
+      <c r="C34" s="32" t="s">
         <v>86</v>
       </c>
       <c r="D34" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37">
         <v>5</v>
       </c>
     </row>
@@ -2066,11 +2143,11 @@
   <conditionalFormatting sqref="B33">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A$1:A$1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C$1:C$1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A29;A35:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30;B34">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
@@ -2084,6 +2161,10 @@
     <hyperlink ref="C32" r:id="rId6" display="mtarmizikubangun@ummaluku.ac.id" tooltip="mailto:mtarmizikubangun@ummaluku.ac.id"/>
     <hyperlink ref="C33" r:id="rId7" display="indrayanisimasima@ummaluku.ac.id" tooltip="mailto:indrayanisimasima@ummaluku.ac.id"/>
     <hyperlink ref="C34" r:id="rId8" display="dosen@ummaluku.ac.id" tooltip="mailto:dosen@ummaluku.ac.id"/>
+    <hyperlink ref="C35" r:id="rId9" display="farisalfadhat@ummaluku.ac.id"/>
+    <hyperlink ref="C36" r:id="rId10" display="andithamrin@ummaluku.ac.id"/>
+    <hyperlink ref="C37" r:id="rId11" display="imamsuprabowo@ummaluku.ac.id" tooltip="mailto:imamsuprabowo@ummaluku.ac.id"/>
+    <hyperlink ref="C28" r:id="rId12" display="morganohiwal@ummaluku.ac.id"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Fix Seeder, import excel (#58)
Co-authored-by: yaufani adam <yaufaniadam@gmail.com>
</commit_message>
<xml_diff>
--- a/database/seeders/data/dosen.xlsx
+++ b/database/seeders/data/dosen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="14960"/>
+    <workbookView windowHeight="14140"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>nidn</t>
   </si>
@@ -242,7 +242,7 @@
     <t>Morga Ohiwal</t>
   </si>
   <si>
-    <t>morgaohiwal@ummaluku.ac.id</t>
+    <t>morganohiwal@ummaluku.ac.id</t>
   </si>
   <si>
     <t>07</t>
@@ -288,6 +288,33 @@
   </si>
   <si>
     <t>dosen@ummaluku.ac.id</t>
+  </si>
+  <si>
+    <t>11111</t>
+  </si>
+  <si>
+    <t>Prof. Faris Al-Fadhat, M.A., Ph.D.</t>
+  </si>
+  <si>
+    <t>farisalfadhat@ummaluku.ac.id</t>
+  </si>
+  <si>
+    <t>22222</t>
+  </si>
+  <si>
+    <t>Dr. Andi Thamrin, SP., M.Si.</t>
+  </si>
+  <si>
+    <t>andithamrin@ummaluku.ac.id</t>
+  </si>
+  <si>
+    <t>33333</t>
+  </si>
+  <si>
+    <t>Dr. Imam Suprabowo, S.Sos.I., M.Pd.I.</t>
+  </si>
+  <si>
+    <t>imamsuprabowo@ummaluku.ac.id</t>
   </si>
 </sst>
 </file>
@@ -300,7 +327,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -312,6 +339,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <charset val="1"/>
       <scheme val="minor"/>
@@ -338,12 +373,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="12"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -986,150 +1019,150 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1189,6 +1222,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1197,15 +1233,17 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1269,12 +1307,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFF9900"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1566,21 +1601,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="18.1625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.45" customWidth="1"/>
-    <col min="3" max="3" width="25.2" customWidth="1"/>
-    <col min="4" max="4" width="16.825" customWidth="1"/>
+    <col min="1" max="1" width="18.1607142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.3214285714286" customWidth="1"/>
+    <col min="3" max="3" width="33.4821428571429" customWidth="1"/>
+    <col min="4" max="4" width="16.8214285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.15" spans="1:4">
+    <row r="1" ht="18.35" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1594,7 +1629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="17" spans="1:4">
+    <row r="2" ht="18" spans="1:4">
       <c r="A2" s="5">
         <v>1221048601</v>
       </c>
@@ -1608,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="17" spans="1:4">
+    <row r="3" ht="18" spans="1:4">
       <c r="A3" s="8">
         <v>1210038801</v>
       </c>
@@ -1622,7 +1657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="17" spans="1:4">
+    <row r="4" ht="18" spans="1:4">
       <c r="A4" s="11">
         <v>1208129501</v>
       </c>
@@ -1636,7 +1671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="17" spans="1:4">
+    <row r="5" ht="18" spans="1:4">
       <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
@@ -1650,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="17" spans="1:4">
+    <row r="6" ht="18" spans="1:4">
       <c r="A6" s="16" t="s">
         <v>13</v>
       </c>
@@ -1748,7 +1783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" ht="17" spans="1:4">
+    <row r="13" ht="18" spans="1:4">
       <c r="A13" s="18">
         <v>1228078512</v>
       </c>
@@ -1762,7 +1797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" ht="17" spans="1:4">
+    <row r="14" ht="18" spans="1:4">
       <c r="A14" s="20">
         <v>1216129001</v>
       </c>
@@ -1776,7 +1811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" ht="17" spans="1:4">
+    <row r="15" ht="18" spans="1:4">
       <c r="A15" s="18">
         <v>1221118201</v>
       </c>
@@ -1790,7 +1825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" ht="17" spans="1:4">
+    <row r="16" ht="18" spans="1:4">
       <c r="A16" s="20">
         <v>1205098702</v>
       </c>
@@ -1804,7 +1839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" ht="17" spans="1:4">
+    <row r="17" ht="18" spans="1:4">
       <c r="A17" s="18">
         <v>12280785122</v>
       </c>
@@ -1818,7 +1853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" ht="17" spans="1:4">
+    <row r="18" ht="18" spans="1:4">
       <c r="A18" s="16" t="s">
         <v>39</v>
       </c>
@@ -1832,7 +1867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" ht="17" spans="1:4">
+    <row r="19" ht="18" spans="1:4">
       <c r="A19" s="14" t="s">
         <v>42</v>
       </c>
@@ -1860,7 +1895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" ht="17" spans="1:4">
+    <row r="21" ht="18" spans="1:4">
       <c r="A21" s="14" t="s">
         <v>48</v>
       </c>
@@ -1874,7 +1909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" ht="17" spans="1:4">
+    <row r="22" ht="18" spans="1:4">
       <c r="A22" s="16" t="s">
         <v>51</v>
       </c>
@@ -1888,7 +1923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" ht="33" spans="1:4">
+    <row r="23" ht="18" spans="1:4">
       <c r="A23" s="14" t="s">
         <v>54</v>
       </c>
@@ -1902,7 +1937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" ht="17" spans="1:4">
+    <row r="24" ht="18" spans="1:4">
       <c r="A24" s="16" t="s">
         <v>57</v>
       </c>
@@ -1916,7 +1951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" ht="17" spans="1:4">
+    <row r="25" ht="18" spans="1:4">
       <c r="A25" s="14" t="s">
         <v>60</v>
       </c>
@@ -1930,7 +1965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" ht="17" spans="1:4">
+    <row r="26" ht="18" spans="1:4">
       <c r="A26" s="16" t="s">
         <v>63</v>
       </c>
@@ -1944,7 +1979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" ht="17" spans="1:4">
+    <row r="27" ht="18" spans="1:4">
       <c r="A27" s="14" t="s">
         <v>66</v>
       </c>
@@ -1958,101 +1993,143 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" ht="17" spans="1:4">
+    <row r="28" ht="18" spans="1:4">
       <c r="A28" s="16" t="s">
         <v>69</v>
       </c>
       <c r="B28" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="25" t="s">
         <v>71</v>
       </c>
       <c r="D28" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="29" ht="17" spans="1:4">
-      <c r="A29" s="25" t="s">
+    <row r="29" ht="18" spans="1:4">
+      <c r="A29" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="28">
+      <c r="D29" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="30" ht="16.8" spans="1:4">
-      <c r="A30" s="33" t="s">
+    <row r="30" spans="1:4">
+      <c r="A30" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="32" t="s">
         <v>77</v>
       </c>
       <c r="D30" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="31" ht="16.8" spans="1:4">
-      <c r="A31" s="33" t="s">
+    <row r="31" spans="1:4">
+      <c r="A31" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="28">
+      <c r="D31" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="32" ht="16.8" spans="1:4">
-      <c r="A32" s="29">
+    <row r="32" spans="1:4">
+      <c r="A32" s="30">
         <v>10</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="32" t="s">
         <v>82</v>
       </c>
       <c r="D32" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="33" ht="16.8" spans="1:4">
-      <c r="A33" s="29">
+    <row r="33" spans="1:4">
+      <c r="A33" s="30">
         <v>11</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="28">
+      <c r="D33" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="34" ht="16.8" spans="1:4">
-      <c r="A34" s="29">
+    <row r="34" spans="1:4">
+      <c r="A34" s="30">
         <v>12</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="31" t="s">
+      <c r="C34" s="32" t="s">
         <v>86</v>
       </c>
       <c r="D34" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37">
         <v>5</v>
       </c>
     </row>
@@ -2066,11 +2143,11 @@
   <conditionalFormatting sqref="B33">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A$1:A$1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C$1:C$1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A29;A35:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30;B34">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
@@ -2084,6 +2161,10 @@
     <hyperlink ref="C32" r:id="rId6" display="mtarmizikubangun@ummaluku.ac.id" tooltip="mailto:mtarmizikubangun@ummaluku.ac.id"/>
     <hyperlink ref="C33" r:id="rId7" display="indrayanisimasima@ummaluku.ac.id" tooltip="mailto:indrayanisimasima@ummaluku.ac.id"/>
     <hyperlink ref="C34" r:id="rId8" display="dosen@ummaluku.ac.id" tooltip="mailto:dosen@ummaluku.ac.id"/>
+    <hyperlink ref="C35" r:id="rId9" display="farisalfadhat@ummaluku.ac.id"/>
+    <hyperlink ref="C36" r:id="rId10" display="andithamrin@ummaluku.ac.id"/>
+    <hyperlink ref="C37" r:id="rId11" display="imamsuprabowo@ummaluku.ac.id" tooltip="mailto:imamsuprabowo@ummaluku.ac.id"/>
+    <hyperlink ref="C28" r:id="rId12" display="morganohiwal@ummaluku.ac.id"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>